<commit_message>
server for both houses updated to actual configuration in lab; scheme / sequence for reading from CSV and providing updated; should be ready for closed loop testing without hardware (SOC_calc is fed back as SOC_measured)
</commit_message>
<xml_diff>
--- a/CoSES/02_Interface_Server/House1/FC_data_series/Test1_Last_Preise.xlsx
+++ b/CoSES/02_Interface_Server/House1/FC_data_series/Test1_Last_Preise.xlsx
@@ -1,22 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23328"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Public\Arbeitsordner_MEMAP\02_Interface_OPCUA_Server\FC_data_series\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Public\A_MEMAPinCoSES_Arbeitsordner\01_MEMAP_platform_servers\CoSES\02_Interface_Server\House1\FC_data_series\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9F9ACE4-CDD7-411C-8862-C97F1D63DFD6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2865" yWindow="2955" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2865" yWindow="2955" windowWidth="21600" windowHeight="11385" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Wärme" sheetId="2" r:id="rId1"/>
     <sheet name="Kosten" sheetId="3" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -35,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="15">
   <si>
     <t>Zeitschritt</t>
   </si>
@@ -85,7 +84,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="ddd"/>
     <numFmt numFmtId="165" formatCode="0.000"/>
@@ -157,7 +156,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -175,7 +174,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="de-DE"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -897,6 +896,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -928,6 +928,7 @@
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
     <c:extLst>
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
@@ -935,7 +936,6 @@
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -973,7 +973,7 @@
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="de-DE"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1692,6 +1692,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1723,6 +1724,7 @@
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
     <c:extLst>
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
@@ -1730,7 +1732,6 @@
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -3225,14 +3226,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{22ABF507-AFCA-496B-A961-3E8F7099BD5D}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N73"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F4" sqref="F4:F12"/>
+      <selection activeCell="F5" sqref="F5:F36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.85546875" customWidth="1"/>
@@ -3267,9 +3268,6 @@
       <c r="A4" s="7"/>
       <c r="B4" s="7"/>
       <c r="C4" s="7"/>
-      <c r="F4">
-        <v>0</v>
-      </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
@@ -3970,9 +3968,7 @@
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A37" s="10" t="s">
-        <v>14</v>
-      </c>
+      <c r="A37" s="10"/>
       <c r="B37" s="10"/>
       <c r="C37" s="10"/>
     </row>
@@ -4243,14 +4239,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7CAF7B51-A847-4EC9-8F79-6CFAC9CF8371}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:N37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4:G36"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5:G36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
   </cols>
@@ -4277,13 +4273,6 @@
       <c r="A4" s="8"/>
       <c r="B4" s="8"/>
       <c r="C4" s="8"/>
-      <c r="F4">
-        <v>9999</v>
-      </c>
-      <c r="G4">
-        <f>F4/100</f>
-        <v>99.99</v>
-      </c>
       <c r="L4" s="7"/>
       <c r="M4" s="7"/>
     </row>

</xml_diff>